<commit_message>
Making the code easier to read.
</commit_message>
<xml_diff>
--- a/data/burnrate-simple.xlsx
+++ b/data/burnrate-simple.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lexar Oct.2023\Lexar\_burnrate-method\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\kanamori\PycharmProjects\BurnRate\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5579DD3E-0635-464A-BECE-A6822BA6521D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7550" xr2:uid="{810016FF-F65A-4EAD-8235-F0CB38A56D92}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="27" r:id="rId1"/>
@@ -35,7 +34,7 @@
     <definedName name="rhop">Propellant!$C$4</definedName>
     <definedName name="to">Propellant!$C$14</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -799,7 +798,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1539,23 +1538,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1594,7 +1593,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C3A0F78-39B1-4685-A4C9-E14B15FEBFB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C3A0F78-39B1-4685-A4C9-E14B15FEBFB0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +1637,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{590E5FB7-BF63-4DD5-9129-792D0E4CA504}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{590E5FB7-BF63-4DD5-9129-792D0E4CA504}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1687,7 +1686,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43A29A6E-B85D-488E-AB80-310C764D36F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{43A29A6E-B85D-488E-AB80-310C764D36F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2012,24 +2011,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CC3F37-FEE3-4C05-A85C-7D12210EEF10}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="10" max="10" width="10.7265625" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" customWidth="1"/>
-    <col min="13" max="13" width="25.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
+    <col min="12" max="12" width="10.875" customWidth="1"/>
+    <col min="13" max="13" width="25.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1"/>
-    <row r="2" spans="2:18" ht="18.5">
+    <row r="2" spans="2:18" ht="18">
       <c r="B2" s="60" t="s">
         <v>72</v>
       </c>
@@ -2047,7 +2046,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="19" thickBot="1">
+    <row r="3" spans="2:18" ht="18.75" thickBot="1">
       <c r="B3" s="63" t="s">
         <v>73</v>
       </c>
@@ -2354,7 +2353,7 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="88" t="s">
+      <c r="B41" s="84" t="s">
         <v>108</v>
       </c>
       <c r="C41" s="4"/>
@@ -2372,7 +2371,7 @@
   </sheetData>
   <sheetProtection password="C7BC" sheet="1" objects="1" scenarios="1"/>
   <hyperlinks>
-    <hyperlink ref="B41" r:id="rId1" xr:uid="{476B00F3-6AB2-49F6-A0FC-B8B1116BF270}"/>
+    <hyperlink ref="B41" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -2381,20 +2380,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85F7DF3-0C74-45C7-A346-A99D58C480E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="B2:O30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="19.90625" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="11.125" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
@@ -2420,7 +2421,8 @@
         <v>19</v>
       </c>
       <c r="C4" s="58">
-        <v>1.6379999999999999</v>
+        <f>0.9*C5</f>
+        <v>1.69452</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -2435,8 +2437,8 @@
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="89">
-        <v>1.655</v>
+      <c r="C5" s="85">
+        <v>1.8828</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -2458,9 +2460,9 @@
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="90">
+      <c r="C6" s="86">
         <f>rhop/C5</f>
-        <v>0.98972809667673711</v>
+        <v>0.9</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>26</v>
@@ -2478,7 +2480,7 @@
     <row r="7" spans="2:15">
       <c r="C7" s="5">
         <f>1000*C4</f>
-        <v>1638</v>
+        <v>1694.52</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -2560,7 +2562,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="58">
-        <v>2433</v>
+        <v>1720</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -2606,7 +2608,7 @@
         <v>71</v>
       </c>
       <c r="C13" s="58">
-        <v>4412</v>
+        <v>2546</v>
       </c>
       <c r="D13" t="s">
         <v>22</v>
@@ -2630,7 +2632,7 @@
       </c>
       <c r="C14" s="2">
         <f>C11*(C13/C12)^2</f>
-        <v>2240.1401119801508</v>
+        <v>527.36015299501412</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -2645,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="58">
-        <v>1.2372000000000001</v>
+        <v>1.133</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>24</v>
@@ -2661,7 +2663,7 @@
       </c>
       <c r="C16" s="2">
         <f>rhop*1000/SQRT(k/rat/to*(2/(k+1))^((k+1)/(k-1)))</f>
-        <v>2231538.9855822367</v>
+        <v>1156185.7156879792</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -2816,20 +2818,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1056873-F91F-4712-8D05-B892E4F7356F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A2:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.90625" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.6328125" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.625" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13">
@@ -2842,12 +2846,12 @@
       </c>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
       <c r="L4" s="16"/>
       <c r="M4" s="16"/>
     </row>
@@ -2876,15 +2880,15 @@
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="54">
-        <v>6.97</v>
-      </c>
-      <c r="F6" s="85" t="s">
+        <v>1.6</v>
+      </c>
+      <c r="F6" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
       <c r="L6" s="11"/>
       <c r="M6" s="17"/>
     </row>
@@ -2899,11 +2903,11 @@
       <c r="E7" s="54">
         <v>5.01</v>
       </c>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
       <c r="L7" s="11"/>
       <c r="M7" s="17"/>
     </row>
@@ -2919,7 +2923,7 @@
       </c>
       <c r="C9" s="29">
         <f>IF(ISBLANK(D6),E6*1000000,D6*6895)</f>
-        <v>6970000</v>
+        <v>1600000</v>
       </c>
       <c r="D9" t="s">
         <v>39</v>
@@ -2933,7 +2937,7 @@
       </c>
       <c r="C10" s="32">
         <f>IF(ISBLANK(D6),E6/E7,D6/D7)</f>
-        <v>1.3912175648702594</v>
+        <v>0.31936127744510984</v>
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="17"/>
@@ -2956,7 +2960,7 @@
       </c>
       <c r="C12" s="32">
         <f>LN(C10)</f>
-        <v>0.33017930967565901</v>
+        <v>-1.1414322858510377</v>
       </c>
       <c r="I12" s="12"/>
       <c r="L12" s="11"/>
@@ -2983,7 +2987,7 @@
       </c>
       <c r="C14" s="3">
         <f>C12/C13</f>
-        <v>1.6114492470860622</v>
+        <v>-5.5707918204844926</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -3014,7 +3018,7 @@
       </c>
       <c r="C17" s="55">
         <f>1-1/C14</f>
-        <v>0.37944058628698885</v>
+        <v>1.1795076951759131</v>
       </c>
       <c r="D17" s="12"/>
       <c r="L17" s="11"/>
@@ -3027,7 +3031,7 @@
       </c>
       <c r="C18" s="55">
         <f>(pone/(knone*con)^m)^(1/m)*1000*1000000^n</f>
-        <v>3.3372869170223423</v>
+        <v>1.7744071502908134</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>11</v>
@@ -3042,7 +3046,7 @@
       </c>
       <c r="C19" s="56">
         <f>C18/25.4*0.006895^n</f>
-        <v>1.9879799761183835E-2</v>
+        <v>1.9713062619308881E-4</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>42</v>
@@ -3084,19 +3088,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0458153C-9D1C-4053-8A4D-E0028ACB01CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="46.7265625" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="46.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
@@ -3116,17 +3122,15 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1"/>
-    <row r="5" spans="2:9" ht="15.5" thickTop="1" thickBot="1">
+    <row r="5" spans="2:9" ht="15.75" thickTop="1" thickBot="1">
       <c r="B5" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="48">
-        <v>82078</v>
-      </c>
+      <c r="C5" s="48"/>
       <c r="D5" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="87" t="s">
+      <c r="E5" s="90" t="s">
         <v>68</v>
       </c>
       <c r="F5" s="33"/>
@@ -3138,11 +3142,13 @@
       <c r="B6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="47"/>
+      <c r="C6" s="47">
+        <v>21.658999999999999</v>
+      </c>
       <c r="D6" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="87"/>
+      <c r="E6" s="90"/>
       <c r="F6" s="33"/>
       <c r="G6" s="33">
         <v>566</v>
@@ -3158,7 +3164,7 @@
       <c r="D7" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="87"/>
+      <c r="E7" s="90"/>
       <c r="F7" s="33"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
@@ -3172,7 +3178,7 @@
       <c r="D8" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="87"/>
+      <c r="E8" s="90"/>
       <c r="F8" s="33">
         <v>5659</v>
       </c>
@@ -3190,37 +3196,37 @@
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
-    <row r="10" spans="2:9" ht="15.5" thickTop="1" thickBot="1">
+    <row r="10" spans="2:9" ht="15.75" thickTop="1" thickBot="1">
       <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="50">
-        <v>0.66100000000000003</v>
-      </c>
+      <c r="C10" s="50"/>
       <c r="D10" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="85" t="s">
+      <c r="E10" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
     </row>
     <row r="11" spans="2:9" ht="15" thickTop="1">
       <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="49"/>
+      <c r="C11" s="49">
+        <v>0.34467999999999999</v>
+      </c>
       <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1">
       <c r="B12" s="1"/>
@@ -3231,43 +3237,43 @@
       <c r="H12" s="33"/>
       <c r="I12" s="33"/>
     </row>
-    <row r="13" spans="2:9" ht="15.5" thickTop="1" thickBot="1">
+    <row r="13" spans="2:9" ht="15.75" thickTop="1" thickBot="1">
       <c r="B13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="50">
-        <v>0.29549999999999998</v>
-      </c>
+      <c r="C13" s="50"/>
       <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="85" t="s">
+      <c r="E13" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickTop="1">
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="49"/>
+      <c r="C14" s="49">
+        <v>12.54</v>
+      </c>
       <c r="D14" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="89"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="1"/>
       <c r="C15" s="53">
         <f>PI()/4*C14^2</f>
-        <v>0</v>
+        <v>123.50511783131016</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -3275,7 +3281,7 @@
         <v>50</v>
       </c>
       <c r="C16" s="45">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="D16" t="s">
         <v>51</v>
@@ -3283,9 +3289,9 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="1"/>
-      <c r="C17" s="43" t="str">
+      <c r="C17" s="43">
         <f>IF($C$6&lt;&gt;"",$C$6,IF($C$7&lt;&gt;"",$C$7,IF($C$8&lt;&gt;"",$C$8,"")))</f>
-        <v/>
+        <v>21.658999999999999</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -3294,7 +3300,7 @@
       </c>
       <c r="C18" s="42">
         <f>IF(ISBLANK(C5),C19*3.2808,C16/C10*386/12*C5*PI()/4*C13^2)</f>
-        <v>2739.2786735979412</v>
+        <v>2546.1678357877058</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>60</v>
@@ -3304,9 +3310,9 @@
       <c r="B19" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="52" t="str">
+      <c r="C19" s="52">
         <f>IF($C$6&lt;&gt;"",$C$6*C15*C16/C11,IF($C$7&lt;&gt;"",$C$7*C15*C16/C11/1000,IF($C$8&lt;&gt;"",$C$8*C15*C16/C11/10,"")))</f>
-        <v/>
+        <v>776.08139349783767</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>61</v>
@@ -3329,7 +3335,7 @@
     <mergeCell ref="E5:E8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" location="Cstar" xr:uid="{F0B37C21-E997-42B6-991B-7122415E665D}"/>
+    <hyperlink ref="B3" r:id="rId1" location="Cstar"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
@@ -3337,17 +3343,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C3E9BF-7585-42F6-A5BC-F58042ED6559}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="9" max="9" width="13.81640625" customWidth="1"/>
+    <col min="9" max="9" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3771,7 +3777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2EF8B97-7825-48D4-A090-2A56B0E96FD8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3779,10 +3785,10 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>